<commit_message>
Updated TODO List for this week
</commit_message>
<xml_diff>
--- a/Documentation/TODO List Fall Quarter.xlsx
+++ b/Documentation/TODO List Fall Quarter.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="229">
   <si>
     <t>Research Tasks</t>
   </si>
@@ -679,6 +679,66 @@
   </si>
   <si>
     <t>Leg Motion Study Animation</t>
+  </si>
+  <si>
+    <t>Taskee</t>
+  </si>
+  <si>
+    <t>Update SolidWorks Model of Robot</t>
+  </si>
+  <si>
+    <t>Robot updated with T-slotted aluminum chassis</t>
+  </si>
+  <si>
+    <t>Lightweight materials research</t>
+  </si>
+  <si>
+    <t>List of potential leg materials/weights</t>
+  </si>
+  <si>
+    <t>Report Tasks</t>
+  </si>
+  <si>
+    <t>Background Section</t>
+  </si>
+  <si>
+    <t>Pedagogical Research</t>
+  </si>
+  <si>
+    <t>Motherboard/Electrical Diagram</t>
+  </si>
+  <si>
+    <t>Clean up electrical section and add full wiring diagram</t>
+  </si>
+  <si>
+    <t>2 Shoulder designs completed</t>
+  </si>
+  <si>
+    <t>2 Leg designs completed</t>
+  </si>
+  <si>
+    <t>Electrical components sized and relative positions mapped out</t>
+  </si>
+  <si>
+    <t>Initial components known and placed for signal conditioning</t>
+  </si>
+  <si>
+    <t>Determine style of Op Amp and number of amplification voltages</t>
+  </si>
+  <si>
+    <t>Update pneumait diagram</t>
+  </si>
+  <si>
+    <t>Updates to background info, Kevin Lee moved</t>
+  </si>
+  <si>
+    <t>Updates to pedagogical research</t>
+  </si>
+  <si>
+    <t>Pneumatic diagram does not have an accumulation tank</t>
+  </si>
+  <si>
+    <t>Animation has realistic gait and determines min/max values</t>
   </si>
 </sst>
 </file>
@@ -1192,10 +1252,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1206,39 +1266,157 @@
     <col min="4" max="16384" width="8.88671875" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="B3" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="B4" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="34" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+      <c r="B5" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="34" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
+      <c r="B6" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="34" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="34" t="s">
+      <c r="B7" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="34" t="s">
         <v>208</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="33" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated TODO list after meeting
</commit_message>
<xml_diff>
--- a/Documentation/TODO List Fall Quarter.xlsx
+++ b/Documentation/TODO List Fall Quarter.xlsx
@@ -12,24 +12,25 @@
     <workbookView xWindow="0" yWindow="132" windowWidth="22980" windowHeight="9468"/>
   </bookViews>
   <sheets>
-    <sheet name="12-3-14 to 12-13-14" sheetId="12" r:id="rId1"/>
-    <sheet name="11-6-14 to 11-13-14" sheetId="10" r:id="rId2"/>
-    <sheet name="11-13-14 to 11-20-14" sheetId="11" r:id="rId3"/>
-    <sheet name="10-30-14 to 11-6-14" sheetId="9" r:id="rId4"/>
-    <sheet name="10-23-14 to 10-30-14" sheetId="8" r:id="rId5"/>
-    <sheet name="10-16-14 to 10-23-14" sheetId="7" r:id="rId6"/>
-    <sheet name="10-9-14 to 10-16-14" sheetId="6" r:id="rId7"/>
-    <sheet name="10-2-14 to 10-9-14" sheetId="5" r:id="rId8"/>
-    <sheet name="9-25-14 to 10-2-14" sheetId="4" r:id="rId9"/>
-    <sheet name="9-18-14 to 9-25-14" sheetId="3" r:id="rId10"/>
-    <sheet name="9-12-14 to 9-18-14" sheetId="1" r:id="rId11"/>
+    <sheet name="12-12-14 to 12-19-14" sheetId="13" r:id="rId1"/>
+    <sheet name="12-3-14 to 12-12-14" sheetId="12" r:id="rId2"/>
+    <sheet name="11-6-14 to 11-13-14" sheetId="10" r:id="rId3"/>
+    <sheet name="11-13-14 to 11-20-14" sheetId="11" r:id="rId4"/>
+    <sheet name="10-30-14 to 11-6-14" sheetId="9" r:id="rId5"/>
+    <sheet name="10-23-14 to 10-30-14" sheetId="8" r:id="rId6"/>
+    <sheet name="10-16-14 to 10-23-14" sheetId="7" r:id="rId7"/>
+    <sheet name="10-9-14 to 10-16-14" sheetId="6" r:id="rId8"/>
+    <sheet name="10-2-14 to 10-9-14" sheetId="5" r:id="rId9"/>
+    <sheet name="9-25-14 to 10-2-14" sheetId="4" r:id="rId10"/>
+    <sheet name="9-18-14 to 9-25-14" sheetId="3" r:id="rId11"/>
+    <sheet name="9-12-14 to 9-18-14" sheetId="1" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="234">
   <si>
     <t>Research Tasks</t>
   </si>
@@ -739,6 +740,21 @@
   </si>
   <si>
     <t>Animation has realistic gait and determines min/max values</t>
+  </si>
+  <si>
+    <t>Derive 27 equations</t>
+  </si>
+  <si>
+    <t>Estimate component masses</t>
+  </si>
+  <si>
+    <t>Shoulder joint design</t>
+  </si>
+  <si>
+    <t>Stress test the microcontroller</t>
+  </si>
+  <si>
+    <t>Look into master slave architecture</t>
   </si>
 </sst>
 </file>
@@ -1252,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1284,90 +1300,27 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
-        <v>203</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
-        <v>204</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="34" t="s">
-        <v>207</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="34" t="s">
-        <v>210</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="34" t="s">
-        <v>212</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1406,17 +1359,6 @@
       </c>
       <c r="C15" s="12" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="34" t="s">
-        <v>224</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -1426,6 +1368,198 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="48.88671875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -1584,7 +1718,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -1814,6 +1948,181 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="56.88671875" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.33203125" style="34" customWidth="1"/>
+    <col min="3" max="3" width="61.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="34"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="34" t="s">
+        <v>205</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="33" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2022,7 +2331,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -2150,7 +2459,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
@@ -2386,7 +2695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -2665,7 +2974,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
@@ -2901,7 +3210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -3103,7 +3412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -3312,196 +3621,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="48.88671875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.21875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="24.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>